<commit_message>
updated with files from ms-v1
</commit_message>
<xml_diff>
--- a/assets/references/aivtf-excel.xlsx
+++ b/assets/references/aivtf-excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pdpc-tanwr\Documents\Observatory\Testing Framework\GenAI\Finalised\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6A313C-1FA7-4BE6-B877-37A364AD1425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36052D8D-2241-447A-B573-540DE5523271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{8350197B-C92E-044C-A1B7-3410D71AC117}"/>
+    <workbookView xWindow="-45" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="13" xr2:uid="{8350197B-C92E-044C-A1B7-3410D71AC117}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Started" sheetId="9" r:id="rId1"/>
@@ -559,14 +559,6 @@
     <t>4.3.1</t>
   </si>
   <si>
-    <t>Document the intended use cases, capabilities, impact and limitations of AI models e.g., via model cards, and approaches for model release
-Include relevant AI actors in the risk identification process
-Process to obtain feedback for risk measurement such as red-teaming and independent evaluation
-Conduct adversarial role-playing exercises red-teaming and chaos testing to identify possible failures 
-State the safeguard requirements (e.g., what are the risks/failures/unacceptable outcomes to mitigate against), safeguard plans (e.g., what are the safeguards, evaluate whether the safeguards are sufficient / working as intended to address the requirements)
-This documentation should be stored and retrieved together with the model artefact, as well as surfaced during a review process before the model is deployed into production</t>
-  </si>
-  <si>
     <t xml:space="preserve">Documentary evidence of risk assessment done for specific use cases. 
 This risk assessment includes documenting* the: 
 - intended use cases, capabilities, and limitations of the AI model (e.g., via model cards)
@@ -579,19 +571,10 @@
     <t>4.3.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Conduct regular evaluation of risks for models that are fine-tuned, or when adapted to new domains or when risks exceeds organisational risk tolerance 
-Ensure fine-tuning does not compromise safety and security controls 
-Develop plan to assess the safeguards after deployment, including how frequent the assessment should occur (e.g., based on time / changes in model capability/performance) and whether the plan is sufficient </t>
-  </si>
-  <si>
     <t>Put in place a process to continuously assess, measure and monitor outcomes and risks, including the identification of new methods and technologies for measurement of risks, as well as  new risks after deployment</t>
   </si>
   <si>
     <t>4.4.1</t>
-  </si>
-  <si>
-    <t>Assign a reviewer who is familiar with the downstream use case of an AI model to review the model post-deployment. This process should include model cards/documentation to ensure alignment between intended use cases at modelling and post-deployment
- Where applicable, share or publish reports detailing the performance, feedback received, and improvements made</t>
   </si>
   <si>
     <t xml:space="preserve">Internal documentation (e.g., log, register or database) / External correspondence </t>
@@ -612,20 +595,10 @@
     <t>4.5.1</t>
   </si>
   <si>
-    <t>Where feasible, use AI models that can produce confidence score together with prediction. Low confidence scores may occur when the data contains values that are outside the range of the training data, or for data regions where there were insufficient training examples to make a robust estimate.
-Implement mechanisms to detect if model might fail or input represents an outlier in terms of training data, e.g., return some "data outlier score" with predictions</t>
-  </si>
-  <si>
     <t>Documentary evidence of assessment of whether the AI system might fail by considering the input features and predicted outcomes to aid communication to stakeholders</t>
   </si>
   <si>
     <t>4.5.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Continuous monitoring of third party systems and fallback plan that monitors the effectiveness of risk controls and mitigation plans 
-Establish proper contracts with third parties, with clear assignment of liability and responsibilities 
-Contingency processes to handle failures or incidents (e.g., arising from third-party data or AI systems that are high risk or data redundancy such as model weights and other system artifacts) or overreliance on third party data and systems 
-</t>
   </si>
   <si>
     <t xml:space="preserve">Internal documentation / External correspondence </t>
@@ -681,11 +654,6 @@
     <t>4.7.1</t>
   </si>
   <si>
-    <t>Document the assessment of the residual risk and provide reasons for the tolerance level
-Risk tracking approaches are considered for settings where AI risks are difficult to assess using currently available measurement techniques or where metrics are not yet available
-For risks difficult to assess or where metrics are not available, put in place risk tracking approaches such as developing a risk reporting matrix, communicating potential risk to affected stakeholders, monitoring risk mitigation plans and reviewing status updates regularly</t>
-  </si>
-  <si>
     <t>Documentary evidence of:
 - implementation of risk tracking approaches
 - assessment of risks that cannot be measured (including explanations such as technological limitations), residual risk and the reasons for the organisation's tolerance for these risks</t>
@@ -695,13 +663,6 @@
   </si>
   <si>
     <t>4.8.1</t>
-  </si>
-  <si>
-    <t>Assess existence or level of harms (e.g., bias, intellectual property infringement)
-Identify content that may violate laws and regulations (e.g., child sexual abuse material (CSAM), non-consensus intimate image (NCII)), inappropriate chemical, biological, radiological and nuclear (CBRN) information), offensive cyber capabilities)
-Implement measures to prevent AI model from generating such content (e.g., guardrails, content filters, human moderation system) and mitigating steps should it happens (e.g.,  integrate feedback into AI system updates)
-Document the mechanisms to prevent AI model from generating content  that violates laws and regulations 
-Monitor and review output regularly for validity, safety, and aligned with socio-cultural norms, trigger alerts for intervention (e.g., use of sentiment analysis to gauge user sentiment)</t>
   </si>
   <si>
     <t xml:space="preserve">Documentary evidence of the organisational policies, mitigation measures if  the content violates the laws and regulations </t>
@@ -739,19 +700,10 @@
     <t>4.10.1</t>
   </si>
   <si>
-    <t xml:space="preserve">For systems that are in experimental stage, put in place a process to document the TEVV considerations. For example, creation of measurement error models for pre-deployment metrics to demonstrate construct validity for each metric.
-Assess the accuracy, quality, reliability and authenticity of output by comparing to ground truth, and conducting adversarial testing to identify vulnerabilities, potential manipulation or misuse of the system
-</t>
-  </si>
-  <si>
     <t>Documentary evidence of TEVV considerations  and policy</t>
   </si>
   <si>
     <t>4.10.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document fact-checking techniques to verify accuracy of information and retention policy to keep history for TEVV
-Use testing techniques to identify AI-generated content and human-generated content </t>
   </si>
   <si>
     <t>Documentary evidence of TEVV considerations and policy</t>
@@ -803,11 +755,6 @@
   </si>
   <si>
     <t>5.3.1</t>
-  </si>
-  <si>
-    <t>Assess and monitor potential security risks of the AI system’s supply chain across its life cycle
-Ensure that suppliers adhere to policy and security standards, or that risks are otherwise appropriately managed
-Consider evaluating supply chain components (e.g. through code checking, or against vulnerability databases)</t>
   </si>
   <si>
     <t>Documentary evidence that supply chain security has been done, these can include:
@@ -1376,10 +1323,6 @@
     <t>8.3.2</t>
   </si>
   <si>
-    <t>Detect presence of personally identifiable information or sensitive data in generated output 
-Implement techniques such as anonymisation, synthetic data generation and privacy enhancing technologies to minimise risks associated with linking AI-generated content back to humans</t>
-  </si>
-  <si>
     <t xml:space="preserve">Documentary evidence of technical tests or detection results, software/developer documentation. Technical tools could include Project Moonshot for red teaming </t>
   </si>
   <si>
@@ -1406,14 +1349,6 @@
     <t>8.5.1</t>
   </si>
   <si>
-    <t>Categorise different types of content associated with third party rights (e.g., copyright, intellectual property)  to be informed on the use of external data
-Implement practices on how third party intellectual property and training data will be used, stored and collected 
-Conduct monitoring of output for privacy risk and data disclosure 
-Implement process to respond to potential intellectual property infringement claims or other rights 
-Educate relevant stakeholders such as third parties on best practices for managing risks 
-Obtain feedback and recommendations from organizational boards or committees when using third-party pre-trained models</t>
-  </si>
-  <si>
     <t>Documentary evidence of:
 - Risk assessment and monitoring related to third party entities have been conducted 
 - Process to respond to third parties on various issues such as infringement claims or other rights 
@@ -1433,14 +1368,6 @@
   </si>
   <si>
     <t>9.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identify acceptable, unacceptable and illegal uses of AI model and output, including criteria for the AI model not respond to (e.g., queries to chatbots)
-Process to engage end users on their expectations and needs (e.g. providing general usage agreements that scope its use)
-Incorporate relevant stakeholders such as end users’ expectations/ needs in the responsible development and use of the AI system
-Implement mechanisms for recourse 
-Compile violations, take-down requests, intellectual property infringement 
-AI policy reviewed regularly to ensure its continued suitability, adequacy and effectiveness, proportional to the identified risks, including making adjustments to organisational roles and components </t>
   </si>
   <si>
     <t>Documentary evidence of 
@@ -1645,11 +1572,6 @@
   </si>
   <si>
     <t>9.12.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Put in place guided flow for documenting (i) the inventory of AI systems and necessary resources (e.g., data, tooling, system &amp; computing and human resources), (ii) risk priorities and (iii) inventory exemptions (e.g. GAI systems embedded into application software). This include inventory of all third party entities. 
-Data include data provenance information such as watermark, signatures, versioning 
-System include bug tracking or external information sharing resource </t>
   </si>
   <si>
     <t xml:space="preserve">Documentary evidence of considerations of resources (e.g., data, tooling, system &amp; computing and human resources) and risk priorities  </t>
@@ -1740,10 +1662,6 @@
     <t>10.3.2</t>
   </si>
   <si>
-    <t>When the AI model is making a decision for which it is significantly unsure of the answer/prediction, consider designing the system to be able to flag these cases and triage them for a human to review
-Monitor and evaluate the instances where human operators or other systems override the GAI's decisions</t>
-  </si>
-  <si>
     <t xml:space="preserve">Documentary evidence of:
 - consideration made in the design of the AI system on its ability to flag instances when it is making a decision for which it is significantly unsure of the answer/prediction, in order that such cases be triaged for a human to review
 - instances where human operators or other systems override the GAI's decisions
@@ -1914,12 +1832,6 @@
   </si>
   <si>
     <t xml:space="preserve">Calculate multiple inferences; and check if the output falls within the accepted limits of the AI system owner  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Complete and submit the Assessment of Materiality to the appropriate parties who are accountable for the AI system (e.g., AI governance committee, AI system owner, and reviewers) and highlight the risks of the proposed AI solution. 
-Document the justifications for decisions on materiality and the application of relevant governance and controls to demonstrate to regulators and auditors that sufficient responsibility has been taken by humans to address potential risks. 
-The materiality assessment could be based on expected use, past uses of AI systems in similar contexts, public incident reports, feedback from those external to the team that developed or deployed the AI system, or other data. This could also be a continuous feedback process between AI system operators and stakeholders
- </t>
   </si>
   <si>
     <r>
@@ -2002,57 +1914,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>For Use</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Understand the AI system's limits, how its output may be utilised and how the AI system interacts with external networks
-Identify potential content provenance harms such as deepfakes 
-Conduct feedback on expectations, concerns, generated content and labels on content. Use feedback to guide design of provenance data-tracking techniques
-Identify methods to trace and analyse the origin and modifications of digital content (e.g., c2pa)
-Provenance data to include an identifier of the service or model that created the content
-Integrate tools to enable real-time monitoring of each instance when content is generated, modified or shared, identify data anomalies and verify authenticity of digital content (e.g., digital signatures)  
-Maintain records of changes to content including content by third parties 
-Implement content provenance management with third parties </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>For evaluation</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Implement evaluation metrics by demographic groups to identify discrepancies in how content provenance mechanisms work across diverse populations 
-Manage statistical bias related to content provenance through techniques such as re-sampling or adversarial training 
-Measure effectiveness and reliability of content provenance methodologies such as watermark
-Apply TEVV practices for content provenance (e.g., probing a system's synthetic data generation capabilities for potential misuse)
-Assess how well solutions address risks or harms </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Documentary evidence of strategy/process undertaken to select fairness metrics that align with the desired outcomes of the AI system's intended application. For example</t>
     </r>
     <r>
@@ -2156,10 +2017,6 @@
     </r>
   </si>
   <si>
-    <t>After models are put into production, put in place mechanisms to review the performance of the models on an ongoing basis, either continuously or at regular intervals.
-Criteria could be time-based (e.g., every 2 years) or event-based (before the launch of a new AI product, after the introduction of new data, operating context has changed due to external circumstances), or when the AI system has undergone substantial modification</t>
-  </si>
-  <si>
     <t>Declaration of transparency on how and where in the decision-making process the AI system is used to complement or replace the human</t>
   </si>
   <si>
@@ -2256,6 +2113,22 @@
 - avoiding changes to the raw data at the source and keeping track of the various stages or transformation steps that are part of the data pipeline for AI model development, preferably as a directed acyclic graph (DAG).</t>
   </si>
   <si>
+    <t>Documentary evidence of monitoring AI system inputs, including:
+- Validating/Monitoring inputs to the model and system for possible attacks and suspicious activity.
+- Monitoring/Limiting rate of queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robustness requires that AI systems maintain its level of performance under any circumstances, including potential changes in their operating environment or the presence of other agents (human or artificial) that may interact with the AI system in an adversarial manner.  This section focuses on the technical robustness of the AI system throughout its AI life cycle, to assess the proper operation of a system as intended by the system owner. This section should be carried out alongside established cybersecurity testing regimes for AI systems, to ensure overall system robustness. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traditional AI - Calculate accuracy metrics at testing time. Add noise to dataset and compare the 2 accuracy metrics (between the dataset with and dataset without noise). The accuracy metric is calculated based on the matching ground truth labels against the predictions.
+Generative AI -  Benchmarking (to compare AI model's performance against time / another model), with datasets that are relevant to the use case. For example, adding noise / perturbate (invariance testing such as synonym, typo, punctuation or adversarial perturbation) to the original prompts in the benchmark and tested against the same metric
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fairness is about designing AI systems that avoid creating or reinforcing unfair bias in the AI system, based on the intended definition of fairness for individuals or groups, that is aligned with the desired outcomes of the AI system. This section focuses on testing the ability of the AI system to align with the intended fairness outcomes, throughout the AI lifecycle. </t>
+  </si>
+  <si>
     <t xml:space="preserve">Identify relevant and/or use-case appropriate benchmarks -  prepare datasets/prompts that include questions or statements that can solicit possible harms including toxic output 
 Document instructions given to AI red-teamers 
 Run benchmarking and redteaming
@@ -2264,6 +2137,65 @@
 Where applicable, share results with relevant stakeholders </t>
   </si>
   <si>
+    <t xml:space="preserve">Complete and submit the Assessment of Materiality to the appropriate parties who are accountable for the AI system (e.g., AI governance committee, AI system owner, and reviewers) and highlight the risks of the proposed AI solution. 
+Document the justifications for decisions on materiality and the application of relevant governance and controls to demonstrate to regulators and auditors that sufficient responsibility has been taken by humans to address potential risks. 
+The materiality assessment could be based on expected use, past uses of AI systems in similar contexts, public incident reports, feedback from those external to the team that developed or deployed the AI system, or other data. This could also be a continuous feedback process between AI system operators and stakeholders
+ </t>
+  </si>
+  <si>
+    <t>Document the intended use cases, capabilities, impact and limitations of AI models e.g., via model cards, and approaches for model release
+Include relevant AI actors in the risk identification process
+Process to obtain feedback for risk measurement such as red-teaming and independent evaluation
+Conduct adversarial role-playing exercises red-teaming and chaos testing to identify possible failures 
+State the safeguard requirements (e.g., what are the risks/failures/unacceptable outcomes to mitigate against), safeguard plans (e.g., what are the safeguards, evaluate whether the safeguards are sufficient / working as intended to address the requirements)
+This documentation should be stored and retrieved together with the model artefact, as well as surfaced during a review process before the model is deployed into production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conduct regular evaluation of risks for models that are fine-tuned, or when adapted to new domains or when risks exceeds organisational risk tolerance 
+Ensure fine-tuning does not compromise safety and security controls 
+Develop plan to assess the safeguards after deployment, including how frequent the assessment should occur (e.g., based on time / changes in model capability/performance) and whether the plan is sufficient </t>
+  </si>
+  <si>
+    <t>Assign a reviewer who is familiar with the downstream use case of an AI model to review the model post-deployment. This process should include model cards/documentation to ensure alignment between intended use cases at modelling and post-deployment
+Where applicable, share or publish reports detailing the performance, feedback received, and improvements made</t>
+  </si>
+  <si>
+    <t>Where feasible, use AI models that can produce confidence score together with prediction. Low confidence scores may occur when the data contains values that are outside the range of the training data, or for data regions where there were insufficient training examples to make a robust estimate.
+Implement mechanisms to detect if model might fail or input represents an outlier in terms of training data, e.g., return some "data outlier score" with predictions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuous monitoring of third party systems and fallback plan that monitors the effectiveness of risk controls and mitigation plans 
+Establish proper contracts with third parties, with clear assignment of liability and responsibilities 
+Contingency processes to handle failures or incidents (e.g., arising from third-party data or AI systems that are high risk or data redundancy such as model weights and other system artifacts) or overreliance on third party data and systems 
+</t>
+  </si>
+  <si>
+    <t>Document the assessment of the residual risk and provide reasons for the tolerance level
+Risk tracking approaches are considered for settings where AI risks are difficult to assess using currently available measurement techniques or where metrics are not yet available
+For risks difficult to assess or where metrics are not available, put in place risk tracking approaches such as developing a risk reporting matrix, communicating potential risk to affected stakeholders, monitoring risk mitigation plans and reviewing status updates regularly</t>
+  </si>
+  <si>
+    <t>Assess existence or level of harms (e.g., bias, intellectual property infringement)
+Identify content that may violate laws and regulations (e.g., child sexual abuse material (CSAM), non-consensus intimate image (NCII)), inappropriate chemical, biological, radiological and nuclear (CBRN) information), offensive cyber capabilities)
+Implement measures to prevent AI model from generating such content (e.g., guardrails, content filters, human moderation system) and mitigating steps should it happens (e.g.,  integrate feedback into AI system updates)
+Document the mechanisms to prevent AI model from generating content  that violates laws and regulations 
+Monitor and review output regularly for validity, safety, and aligned with socio-cultural norms, trigger alerts for intervention (e.g., use of sentiment analysis to gauge user sentiment)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For systems that are in experimental stage, put in place a process to document the TEVV considerations. For example, creation of measurement error models for pre-deployment metrics to demonstrate construct validity for each metric.
+Assess the accuracy, quality, reliability and authenticity of output by comparing to ground truth, and conducting adversarial testing to identify vulnerabilities, potential manipulation or misuse of the system
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document fact-checking techniques to verify accuracy of information and retention policy to keep history for TEVV
+Use testing techniques to identify AI-generated content and human-generated content </t>
+  </si>
+  <si>
+    <t>Assess and monitor potential security risks of the AI system’s supply chain across its life cycle
+Ensure that suppliers adhere to policy and security standards, or that risks are otherwise appropriately managed
+Consider evaluating supply chain components (e.g. through code checking, or against vulnerability databases)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identify relevant and/or use-case appropriate benchmarks - prepare datasets/prompts that include questions or statements that can solicit possible harms including toxic output against individuals or groups
 Document instructions given to AI red-teamers 
 Run benchmarking and redteaming
@@ -2271,14 +2203,29 @@
 Where applicable, share results with relevant stakeholders </t>
   </si>
   <si>
+    <t>Detect presence of personally identifiable information or sensitive data in generated output 
+Implement techniques such as anonymisation, synthetic data generation and privacy enhancing technologies to minimise risks associated with linking AI-generated content back to humans</t>
+  </si>
+  <si>
+    <t>Categorise different types of content associated with third party rights (e.g., copyright, intellectual property)  to be informed on the use of external data
+Implement practices on how third party intellectual property and training data will be used, stored and collected 
+Conduct monitoring of output for privacy risk and data disclosure 
+Implement process to respond to potential intellectual property infringement claims or other rights 
+Educate relevant stakeholders such as third parties on best practices for managing risks 
+Obtain feedback and recommendations from organizational boards or committees when using third-party pre-trained models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify acceptable, unacceptable and illegal uses of AI model and output, including criteria for the AI model not respond to (e.g., queries to chatbots)
+Process to engage end users on their expectations and needs (e.g. providing general usage agreements that scope its use)
+Incorporate relevant stakeholders such as end users’ expectations/ needs in the responsible development and use of the AI system
+Implement mechanisms for recourse 
+Compile violations, take-down requests, intellectual property infringement 
+AI policy reviewed regularly to ensure its continued suitability, adequacy and effectiveness, proportional to the identified risks, including making adjustments to organisational roles and components </t>
+  </si>
+  <si>
     <t xml:space="preserve">For organisations who are using AI across departments, establish teams or AI governance committee that comprises representatives from data science, technology, risk, and product to facilitate cross-departmental oversight for the lifecycle governance of AI systems 
 If it's not practical to have cross-department oversight, integrate accountability of the use of AI into existing risk or compliance structures
 For systems with national security risks, involve relevant stakeholders </t>
-  </si>
-  <si>
-    <t>Documentary evidence of monitoring AI system inputs, including:
-- Validating/Monitoring inputs to the model and system for possible attacks and suspicious activity.
-- Monitoring/Limiting rate of queries</t>
   </si>
   <si>
     <t>Responsibilities and obligations are clearly communicated to all parties related to the AI system
@@ -2290,15 +2237,68 @@
 - transparency artifacts (e.g., model and system cards) for third party models</t>
   </si>
   <si>
-    <t xml:space="preserve">Robustness requires that AI systems maintain its level of performance under any circumstances, including potential changes in their operating environment or the presence of other agents (human or artificial) that may interact with the AI system in an adversarial manner.  This section focuses on the technical robustness of the AI system throughout its AI life cycle, to assess the proper operation of a system as intended by the system owner. This section should be carried out alongside established cybersecurity testing regimes for AI systems, to ensure overall system robustness. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Traditional AI - Calculate accuracy metrics at testing time. Add noise to dataset and compare the 2 accuracy metrics (between the dataset with and dataset without noise). The accuracy metric is calculated based on the matching ground truth labels against the predictions.
-Generative AI -  Benchmarking (to compare AI model's performance against time / another model), with datasets that are relevant to the use case. For example, adding noise / perturbate (invariance testing such as synonym, typo, punctuation or adversarial perturbation) to the original prompts in the benchmark and tested against the same metric
+    <t xml:space="preserve">Put in place guided flow for documenting (i) the inventory of AI systems and necessary resources (e.g., data, tooling, system &amp; computing and human resources), (ii) risk priorities and (iii) inventory exemptions (e.g. GAI systems embedded into application software). This include inventory of all third party entities. 
+Data include data provenance information such as watermark, signatures, versioning 
+System include bug tracking or external information sharing resource </t>
+  </si>
+  <si>
+    <t>When the AI model is making a decision for which it is significantly unsure of the answer/prediction, consider designing the system to be able to flag these cases and triage them for a human to review
+Monitor and evaluate the instances where human operators or other systems override the GAI's decisions</t>
+  </si>
+  <si>
+    <t>After models are put into production, put in place mechanisms to review the performance of the models on an ongoing basis, either continuously or at regular intervals.
+Criteria could be time-based (e.g., every 2 years) or event-based (before the launch of a new AI product, after the introduction of new data, operating context has changed due to external circumstances), or when the AI system has undergone substantial modification</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>For Use</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+Understand the AI system's limits, how its output may be utilised and how the AI system interacts with external networks
+Identify potential content provenance harms such as deepfakes 
+Conduct feedback on expectations, concerns, generated content and labels on content. Use feedback to guide design of provenance data-tracking techniques
+Identify methods to trace and analyse the origin and modifications of digital content (e.g., c2pa)
+Provenance data to include an identifier of the service or model that created the content
+Integrate tools to enable real-time monitoring of each instance when content is generated, modified or shared, identify data anomalies and verify authenticity of digital content (e.g., digital signatures)  
+Maintain records of changes to content including content by third parties 
+Implement content provenance management with third parties </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">For evaluation
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fairness is about designing AI systems that avoid creating or reinforcing unfair bias in the AI system, based on the intended definition of fairness for individuals or groups, that is aligned with the desired outcomes of the AI system. This section focuses on testing the ability of the AI system to align with the intended fairness outcomes, throughout the AI lifecycle. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Implement evaluation metrics by demographic groups to identify discrepancies in how content provenance mechanisms work across diverse populations 
+Manage statistical bias related to content provenance through techniques such as re-sampling or adversarial training 
+Measure effectiveness and reliability of content provenance methodologies such as watermark
+Apply TEVV practices for content provenance (e.g., probing a system's synthetic data generation capabilities for potential misuse)
+Assess how well solutions address risks or harms </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4153,7 +4153,7 @@
   </sheetPr>
   <dimension ref="C2:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -4210,7 +4210,7 @@
         <v>6</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="K5" s="40" t="s">
         <v>7</v>
@@ -4243,8 +4243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F3E10A-28C2-4086-BFF9-7908DE9D3DB6}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -4263,7 +4263,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4276,7 +4276,7 @@
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -4289,7 +4289,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>524</v>
+        <v>501</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -4330,13 +4330,13 @@
         <v>6</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="73" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="I5" s="73" t="s">
         <v>52</v>
@@ -4350,24 +4350,24 @@
         <v>81</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="F6" s="59" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="H6" s="57"/>
       <c r="I6" s="60"/>
     </row>
-    <row r="7" spans="1:9" ht="155" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A7" s="63">
         <v>7.2</v>
       </c>
@@ -4375,13 +4375,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F7" s="59" t="s">
         <v>79</v>
@@ -4422,13 +4422,13 @@
         <v>6</v>
       </c>
       <c r="F9" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G9" s="73" t="s">
         <v>7</v>
       </c>
       <c r="H9" s="73" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="I9" s="73" t="s">
         <v>52</v>
@@ -4442,19 +4442,19 @@
         <v>81</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="H10" s="57"/>
       <c r="I10" s="60"/>
@@ -4467,19 +4467,19 @@
         <v>51</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="F11" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="H11" s="57"/>
       <c r="I11" s="60"/>
@@ -4492,19 +4492,19 @@
         <v>81</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E12" s="59" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G12" s="59" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
       <c r="H12" s="57"/>
       <c r="I12" s="60"/>
@@ -4517,19 +4517,19 @@
         <v>81</v>
       </c>
       <c r="C13" s="93" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="E13" s="59" t="s">
-        <v>490</v>
+        <v>472</v>
       </c>
       <c r="F13" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="H13" s="57"/>
       <c r="I13" s="60"/>
@@ -4543,21 +4543,21 @@
       </c>
       <c r="C14" s="93"/>
       <c r="D14" s="64" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="F14" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="60"/>
     </row>
-    <row r="15" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="124" x14ac:dyDescent="0.35">
       <c r="A15" s="63">
         <v>7.8</v>
       </c>
@@ -4565,19 +4565,19 @@
         <v>51</v>
       </c>
       <c r="C15" s="59" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="F15" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G15" s="59" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="H15" s="57"/>
       <c r="I15" s="60"/>
@@ -4590,44 +4590,44 @@
         <v>51</v>
       </c>
       <c r="C16" s="59" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G16" s="59" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="H16" s="57"/>
       <c r="I16" s="60"/>
     </row>
     <row r="17" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A17" s="74" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="B17" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C17" s="59" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E17" s="59" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F17" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G17" s="59" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="H17" s="57"/>
       <c r="I17" s="60"/>
@@ -4640,19 +4640,19 @@
         <v>51</v>
       </c>
       <c r="C18" s="59" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="E18" s="81" t="s">
-        <v>489</v>
+        <v>471</v>
       </c>
       <c r="F18" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G18" s="59" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="H18" s="57"/>
       <c r="I18" s="60"/>
@@ -4695,8 +4695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02D9A3D-BDF8-4989-AAEF-344452A0B78E}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -4715,7 +4715,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4728,7 +4728,7 @@
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -4741,7 +4741,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -4782,7 +4782,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>7</v>
@@ -4802,24 +4802,24 @@
         <v>51</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:9" ht="263.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="279" x14ac:dyDescent="0.35">
       <c r="A7" s="65">
         <v>8.1999999999999993</v>
       </c>
@@ -4827,19 +4827,19 @@
         <v>51</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -4852,40 +4852,40 @@
         <v>51</v>
       </c>
       <c r="C8" s="94" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
     </row>
-    <row r="9" spans="1:9" ht="93" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A9" s="97"/>
       <c r="B9" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="95"/>
       <c r="D9" s="19" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>345</v>
+        <v>515</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -4898,24 +4898,24 @@
         <v>51</v>
       </c>
       <c r="C10" s="66" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="310" x14ac:dyDescent="0.35">
       <c r="A11" s="65">
         <v>8.5</v>
       </c>
@@ -4923,19 +4923,19 @@
         <v>51</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>353</v>
+        <v>516</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
@@ -4976,8 +4976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BC4367-3AB0-4B1C-8E66-0CE4E89A324A}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -4996,7 +4996,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5009,7 +5009,7 @@
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -5022,7 +5022,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5063,7 +5063,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>7</v>
@@ -5075,7 +5075,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="248" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="325.5" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>9.1</v>
       </c>
@@ -5083,19 +5083,19 @@
         <v>51</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>360</v>
+        <v>517</v>
       </c>
       <c r="F6" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="61" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
@@ -5108,19 +5108,19 @@
         <v>51</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="F7" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="H7" s="59"/>
       <c r="I7" s="59"/>
@@ -5133,19 +5133,19 @@
         <v>51</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="D8" s="62" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="G8" s="61" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="H8" s="59"/>
       <c r="I8" s="59"/>
@@ -5158,19 +5158,19 @@
         <v>51</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="D9" s="62" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="F9" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G9" s="61" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="H9" s="59"/>
       <c r="I9" s="59"/>
@@ -5183,19 +5183,19 @@
         <v>51</v>
       </c>
       <c r="C10" s="91" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="D10" s="62" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="F10" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="H10" s="59"/>
       <c r="I10" s="59"/>
@@ -5207,16 +5207,16 @@
       </c>
       <c r="C11" s="91"/>
       <c r="D11" s="62" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="H11" s="59"/>
       <c r="I11" s="59"/>
@@ -5228,16 +5228,16 @@
       </c>
       <c r="C12" s="91"/>
       <c r="D12" s="62" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="F12" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G12" s="61" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="H12" s="59"/>
       <c r="I12" s="59"/>
@@ -5249,16 +5249,16 @@
       </c>
       <c r="C13" s="91"/>
       <c r="D13" s="62" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>491</v>
+        <v>473</v>
       </c>
       <c r="F13" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="H13" s="59"/>
       <c r="I13" s="59"/>
@@ -5271,19 +5271,19 @@
         <v>51</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="D14" s="62" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="H14" s="59"/>
       <c r="I14" s="59"/>
@@ -5296,19 +5296,19 @@
         <v>51</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="D15" s="62" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F15" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G15" s="61" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="H15" s="59"/>
       <c r="I15" s="59"/>
@@ -5321,19 +5321,19 @@
         <v>51</v>
       </c>
       <c r="C16" s="61" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="D16" s="62" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="F16" s="61" t="s">
         <v>90</v>
       </c>
       <c r="G16" s="61" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="H16" s="59"/>
       <c r="I16" s="59"/>
@@ -5346,19 +5346,19 @@
         <v>51</v>
       </c>
       <c r="C17" s="91" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="D17" s="62" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="E17" s="61" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="F17" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="H17" s="59"/>
       <c r="I17" s="59"/>
@@ -5370,91 +5370,91 @@
       </c>
       <c r="C18" s="91"/>
       <c r="D18" s="62" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="F18" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="61" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="H18" s="59"/>
       <c r="I18" s="59"/>
     </row>
-    <row r="19" spans="1:9" ht="372" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="387.5" x14ac:dyDescent="0.35">
       <c r="A19" s="84" t="s">
-        <v>507</v>
+        <v>488</v>
       </c>
       <c r="B19" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="D19" s="62" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>492</v>
+        <v>474</v>
       </c>
       <c r="F19" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="61" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="H19" s="59"/>
       <c r="I19" s="59"/>
     </row>
     <row r="20" spans="1:9" ht="124" x14ac:dyDescent="0.35">
       <c r="A20" s="84" t="s">
-        <v>508</v>
+        <v>489</v>
       </c>
       <c r="B20" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="D20" s="62" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="E20" s="61" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="F20" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G20" s="61" t="s">
-        <v>410</v>
+        <v>397</v>
       </c>
       <c r="H20" s="59"/>
       <c r="I20" s="59"/>
     </row>
-    <row r="21" spans="1:9" ht="155" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="186" x14ac:dyDescent="0.35">
       <c r="A21" s="84" t="s">
-        <v>509</v>
+        <v>490</v>
       </c>
       <c r="B21" s="59" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="61" t="s">
-        <v>411</v>
+        <v>398</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>412</v>
+        <v>399</v>
       </c>
       <c r="E21" s="61" t="s">
-        <v>413</v>
+        <v>520</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G21" s="61" t="s">
-        <v>414</v>
+        <v>400</v>
       </c>
       <c r="H21" s="59"/>
       <c r="I21" s="59"/>
@@ -5497,8 +5497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F3AFAE-C90E-4126-8532-3C50448D7408}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -5517,7 +5517,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>415</v>
+        <v>401</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>416</v>
+        <v>402</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -5543,7 +5543,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>417</v>
+        <v>403</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5584,7 +5584,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>7</v>
@@ -5604,19 +5604,19 @@
         <v>51</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>420</v>
+        <v>406</v>
       </c>
       <c r="F6" s="61" t="s">
-        <v>421</v>
+        <v>407</v>
       </c>
       <c r="G6" s="61" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
@@ -5629,19 +5629,19 @@
         <v>51</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>423</v>
+        <v>409</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>424</v>
+        <v>410</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>425</v>
+        <v>411</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="H7" s="59"/>
       <c r="I7" s="59"/>
@@ -5653,16 +5653,16 @@
       </c>
       <c r="C8" s="91"/>
       <c r="D8" s="62" t="s">
-        <v>427</v>
+        <v>413</v>
       </c>
       <c r="E8" s="61" t="s">
-        <v>428</v>
+        <v>414</v>
       </c>
       <c r="F8" s="61" t="s">
-        <v>429</v>
+        <v>415</v>
       </c>
       <c r="G8" s="61" t="s">
-        <v>430</v>
+        <v>416</v>
       </c>
       <c r="H8" s="59"/>
       <c r="I8" s="59"/>
@@ -5675,19 +5675,19 @@
         <v>51</v>
       </c>
       <c r="C9" s="91" t="s">
-        <v>431</v>
+        <v>417</v>
       </c>
       <c r="D9" s="62" t="s">
-        <v>432</v>
+        <v>418</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>433</v>
+        <v>419</v>
       </c>
       <c r="F9" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G9" s="61" t="s">
-        <v>513</v>
+        <v>494</v>
       </c>
       <c r="H9" s="59"/>
       <c r="I9" s="59"/>
@@ -5699,16 +5699,16 @@
       </c>
       <c r="C10" s="91"/>
       <c r="D10" s="62" t="s">
-        <v>434</v>
+        <v>420</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>435</v>
+        <v>521</v>
       </c>
       <c r="F10" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="H10" s="59"/>
       <c r="I10" s="59"/>
@@ -5720,16 +5720,16 @@
       </c>
       <c r="C11" s="91"/>
       <c r="D11" s="62" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="F11" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="H11" s="59"/>
       <c r="I11" s="59"/>
@@ -5742,24 +5742,24 @@
         <v>51</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="D12" s="62" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
       <c r="E12" s="61" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="F12" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G12" s="61" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="H12" s="59"/>
       <c r="I12" s="59"/>
     </row>
-    <row r="13" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A13" s="62">
         <v>10.5</v>
       </c>
@@ -5767,19 +5767,19 @@
         <v>51</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
       <c r="D13" s="62" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>493</v>
+        <v>522</v>
       </c>
       <c r="F13" s="61" t="s">
         <v>90</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
       <c r="H13" s="59"/>
       <c r="I13" s="59"/>
@@ -5792,19 +5792,19 @@
         <v>51</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
       <c r="D14" s="62" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>494</v>
+        <v>475</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
       <c r="H14" s="59"/>
       <c r="I14" s="59"/>
@@ -5847,8 +5847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388FBDCA-22C9-4F2B-B7E6-3A2316F443F5}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -5867,7 +5867,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5880,7 +5880,7 @@
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -5893,7 +5893,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -5934,7 +5934,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>7</v>
@@ -5954,19 +5954,19 @@
         <v>51</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
       <c r="D6" s="62" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>495</v>
+        <v>476</v>
       </c>
       <c r="F6" s="61" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="G6" s="61" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="59"/>
@@ -5979,19 +5979,19 @@
         <v>51</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="D7" s="62" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="E7" s="61" t="s">
-        <v>496</v>
+        <v>477</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G7" s="61" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="H7" s="59"/>
       <c r="I7" s="59"/>
@@ -6129,7 +6129,7 @@
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="2:7" ht="20" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" ht="40" x14ac:dyDescent="0.35">
       <c r="C3" s="2" t="s">
         <v>61</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="76" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="D19" s="25">
         <f>COUNTA('5. Security'!H6:H19)</f>
@@ -6317,7 +6317,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="76" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="D22" s="25">
         <f>COUNTA('6. Robustness'!H6,'6. Robustness'!H9:H17)</f>
@@ -6349,7 +6349,7 @@
         <v>7</v>
       </c>
       <c r="C25" s="76" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="D25" s="25">
         <f>COUNTA('7. Fairness'!H6:H7,'7. Fairness'!H10:H18)</f>
@@ -6381,7 +6381,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="76" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D28" s="25">
         <f>COUNTA('8. Data Governance'!H6:H11)</f>
@@ -6413,7 +6413,7 @@
         <v>9</v>
       </c>
       <c r="C31" s="76" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="D31" s="25">
         <f>COUNTA('9. Accountability'!H6:H21)</f>
@@ -6445,7 +6445,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="76" t="s">
-        <v>479</v>
+        <v>464</v>
       </c>
       <c r="D34" s="25">
         <f>COUNTA('10. Human agency'!H6:H14)</f>
@@ -6477,7 +6477,7 @@
         <v>11</v>
       </c>
       <c r="C37" s="76" t="s">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="D37" s="25">
         <f>COUNTA('11. Inclusive growth'!H6:H7)</f>
@@ -6557,8 +6557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865DB527-8B2A-AC47-987F-12E7458636DC}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -6644,7 +6644,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>7</v>
@@ -6691,7 +6691,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>499</v>
+        <v>480</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>36</v>
@@ -6712,13 +6712,13 @@
         <v>18</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>498</v>
+        <v>479</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>497</v>
+        <v>478</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -6765,7 +6765,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" ht="263.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" s="10" customFormat="1" ht="279" x14ac:dyDescent="0.35">
       <c r="A11" s="85"/>
       <c r="B11" s="14" t="s">
         <v>51</v>
@@ -6848,13 +6848,13 @@
         <v>24</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>501</v>
+        <v>482</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
@@ -6996,8 +6996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1990E96F-B4B3-0B47-BF9C-A7515C6611BA}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -7083,13 +7083,13 @@
         <v>6</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>52</v>
@@ -7103,7 +7103,7 @@
         <v>81</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>481</v>
+        <v>466</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>77</v>
@@ -7150,7 +7150,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>7</v>
@@ -7170,10 +7170,10 @@
         <v>51</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>514</v>
+        <v>495</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>502</v>
+        <v>483</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>82</v>
@@ -7182,7 +7182,7 @@
         <v>37</v>
       </c>
       <c r="G9" s="55" t="s">
-        <v>474</v>
+        <v>459</v>
       </c>
       <c r="H9" s="57"/>
       <c r="I9" s="14"/>
@@ -7238,8 +7238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4185AA65-0084-4282-B491-6897146F13BB}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -7325,7 +7325,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>7</v>
@@ -7502,16 +7502,16 @@
         <v>110</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>503</v>
+        <v>484</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>482</v>
+        <v>467</v>
       </c>
       <c r="F13" s="42" t="s">
         <v>90</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>515</v>
+        <v>496</v>
       </c>
       <c r="H13" s="42"/>
       <c r="I13" s="14"/>
@@ -7584,32 +7584,32 @@
         <v>90</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>516</v>
+        <v>497</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A17" s="82" t="s">
-        <v>504</v>
+        <v>485</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
@@ -7619,22 +7619,22 @@
         <v>3.11</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>469</v>
+        <v>454</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
@@ -7644,22 +7644,22 @@
         <v>3.12</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>505</v>
+        <v>486</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>470</v>
+        <v>455</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>471</v>
+        <v>456</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>472</v>
+        <v>457</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>90</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>473</v>
+        <v>458</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -7714,8 +7714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{070DAC1C-7564-4E78-835E-ED819C263821}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -7801,7 +7801,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>506</v>
+        <v>487</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>7</v>
@@ -7813,7 +7813,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="279" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="372" x14ac:dyDescent="0.35">
       <c r="A6" s="62">
         <v>4.0999999999999996</v>
       </c>
@@ -7827,7 +7827,7 @@
         <v>125</v>
       </c>
       <c r="E6" s="61" t="s">
-        <v>517</v>
+        <v>502</v>
       </c>
       <c r="F6" s="61" t="s">
         <v>79</v>
@@ -7868,13 +7868,13 @@
         <v>6</v>
       </c>
       <c r="F8" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G8" s="73" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="73" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="I8" s="73" t="s">
         <v>52</v>
@@ -7894,13 +7894,13 @@
         <v>128</v>
       </c>
       <c r="E9" s="61" t="s">
-        <v>483</v>
+        <v>503</v>
       </c>
       <c r="F9" s="61" t="s">
         <v>129</v>
       </c>
       <c r="G9" s="61" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="H9" s="59"/>
       <c r="I9" s="60"/>
@@ -7919,28 +7919,28 @@
         <v>131</v>
       </c>
       <c r="E10" s="61" t="s">
-        <v>132</v>
+        <v>504</v>
       </c>
       <c r="F10" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H10" s="59"/>
       <c r="I10" s="60"/>
     </row>
-    <row r="11" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
       <c r="A11" s="90"/>
       <c r="B11" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="91"/>
       <c r="D11" s="62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E11" s="61" t="s">
-        <v>135</v>
+        <v>505</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>37</v>
@@ -7957,24 +7957,24 @@
         <v>51</v>
       </c>
       <c r="C12" s="61" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="61" t="s">
+        <v>506</v>
+      </c>
+      <c r="F12" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="D12" s="62" t="s">
+      <c r="G12" s="61" t="s">
         <v>137</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" s="61" t="s">
-        <v>139</v>
-      </c>
-      <c r="G12" s="61" t="s">
-        <v>140</v>
       </c>
       <c r="H12" s="59"/>
       <c r="I12" s="60"/>
     </row>
-    <row r="13" spans="1:9" ht="139.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="155" x14ac:dyDescent="0.35">
       <c r="A13" s="90">
         <v>4.5</v>
       </c>
@@ -7982,40 +7982,40 @@
         <v>51</v>
       </c>
       <c r="C13" s="91" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D13" s="62" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E13" s="61" t="s">
-        <v>143</v>
+        <v>507</v>
       </c>
       <c r="F13" s="61" t="s">
         <v>90</v>
       </c>
       <c r="G13" s="61" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="H13" s="59"/>
       <c r="I13" s="60"/>
     </row>
-    <row r="14" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A14" s="90"/>
       <c r="B14" s="61" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="91"/>
       <c r="D14" s="62" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E14" s="61" t="s">
-        <v>146</v>
+        <v>508</v>
       </c>
       <c r="F14" s="61" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G14" s="61" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="H14" s="59"/>
       <c r="I14" s="60"/>
@@ -8028,19 +8028,19 @@
         <v>51</v>
       </c>
       <c r="C15" s="91" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D15" s="62" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E15" s="61" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F15" s="61" t="s">
         <v>90</v>
       </c>
       <c r="G15" s="61" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H15" s="59"/>
       <c r="I15" s="60"/>
@@ -8052,16 +8052,16 @@
       </c>
       <c r="C16" s="91"/>
       <c r="D16" s="62" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E16" s="61" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F16" s="61" t="s">
         <v>90</v>
       </c>
       <c r="G16" s="61" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H16" s="59"/>
       <c r="I16" s="60"/>
@@ -8073,16 +8073,16 @@
       </c>
       <c r="C17" s="91"/>
       <c r="D17" s="62" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E17" s="80" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="F17" s="61" t="s">
         <v>90</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H17" s="59"/>
       <c r="I17" s="60"/>
@@ -8094,21 +8094,21 @@
       </c>
       <c r="C18" s="91"/>
       <c r="D18" s="62" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E18" s="61" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F18" s="61" t="s">
         <v>95</v>
       </c>
       <c r="G18" s="61" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="H18" s="59"/>
       <c r="I18" s="60"/>
     </row>
-    <row r="19" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
       <c r="A19" s="62">
         <v>4.7</v>
       </c>
@@ -8116,24 +8116,24 @@
         <v>51</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D19" s="62" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E19" s="61" t="s">
-        <v>163</v>
+        <v>509</v>
       </c>
       <c r="F19" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="61" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H19" s="59"/>
       <c r="I19" s="60"/>
     </row>
-    <row r="20" spans="1:9" ht="263.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="341" x14ac:dyDescent="0.35">
       <c r="A20" s="62">
         <v>4.8</v>
       </c>
@@ -8141,24 +8141,24 @@
         <v>11</v>
       </c>
       <c r="C20" s="61" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D20" s="62" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E20" s="61" t="s">
-        <v>167</v>
+        <v>510</v>
       </c>
       <c r="F20" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G20" s="61" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="H20" s="59"/>
       <c r="I20" s="60"/>
     </row>
-    <row r="21" spans="1:9" ht="325.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A21" s="90">
         <v>4.9000000000000004</v>
       </c>
@@ -8166,86 +8166,86 @@
         <v>11</v>
       </c>
       <c r="C21" s="91" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D21" s="62" t="s">
-        <v>170</v>
-      </c>
-      <c r="E21" s="61" t="s">
-        <v>486</v>
+        <v>163</v>
+      </c>
+      <c r="E21" s="80" t="s">
+        <v>523</v>
       </c>
       <c r="F21" s="61" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G21" s="61" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="H21" s="59"/>
       <c r="I21" s="60"/>
     </row>
-    <row r="22" spans="1:9" ht="201.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="263.5" x14ac:dyDescent="0.35">
       <c r="A22" s="90"/>
       <c r="B22" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="91"/>
       <c r="D22" s="62" t="s">
-        <v>172</v>
-      </c>
-      <c r="E22" s="61" t="s">
-        <v>487</v>
+        <v>165</v>
+      </c>
+      <c r="E22" s="80" t="s">
+        <v>524</v>
       </c>
       <c r="F22" s="61" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G22" s="61" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H22" s="59"/>
       <c r="I22" s="60"/>
     </row>
     <row r="23" spans="1:9" ht="279" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="90" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B23" s="61" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="91" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D23" s="62" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="E23" s="61" t="s">
-        <v>176</v>
+        <v>511</v>
       </c>
       <c r="F23" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G23" s="61" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H23" s="59"/>
       <c r="I23" s="60"/>
     </row>
-    <row r="24" spans="1:9" ht="62" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A24" s="90"/>
       <c r="B24" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C24" s="91"/>
       <c r="D24" s="62" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E24" s="61" t="s">
-        <v>179</v>
+        <v>512</v>
       </c>
       <c r="F24" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G24" s="61" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="H24" s="59"/>
       <c r="I24" s="60"/>
@@ -8297,8 +8297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78ADE93-57C3-40CD-BAC3-A27EC910F7A0}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -8317,7 +8317,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8330,7 +8330,7 @@
     </row>
     <row r="2" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -8343,7 +8343,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -8384,7 +8384,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>7</v>
@@ -8404,19 +8404,19 @@
         <v>51</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F6" s="59" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H6" s="14"/>
       <c r="I6" s="63"/>
@@ -8429,19 +8429,19 @@
         <v>51</v>
       </c>
       <c r="C7" s="59" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="D7" s="64" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F7" s="59" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="G7" s="59" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="63"/>
@@ -8454,19 +8454,19 @@
         <v>51</v>
       </c>
       <c r="C8" s="59" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>194</v>
+        <v>513</v>
       </c>
       <c r="F8" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G8" s="59" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H8" s="14"/>
       <c r="I8" s="63"/>
@@ -8479,19 +8479,19 @@
         <v>51</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="F9" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G9" s="59" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="63"/>
@@ -8504,19 +8504,19 @@
         <v>51</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F10" s="59" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="63"/>
@@ -8529,19 +8529,19 @@
         <v>51</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>478</v>
+        <v>463</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="F11" s="59" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="63"/>
@@ -8554,19 +8554,19 @@
         <v>51</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="E12" s="59" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="G12" s="59" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="63"/>
@@ -8579,19 +8579,19 @@
         <v>51</v>
       </c>
       <c r="C13" s="59" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E13" s="59" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="F13" s="59" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="63"/>
@@ -8604,49 +8604,49 @@
         <v>51</v>
       </c>
       <c r="C14" s="59" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="F14" s="59" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="63"/>
     </row>
     <row r="15" spans="1:9" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A15" s="83" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="B15" s="61" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="59" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="F15" s="59" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G15" s="59" t="s">
-        <v>520</v>
+        <v>498</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="63"/>
     </row>
-    <row r="16" spans="1:9" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="186" x14ac:dyDescent="0.35">
       <c r="A16" s="63">
         <v>5.1100000000000003</v>
       </c>
@@ -8654,19 +8654,19 @@
         <v>51</v>
       </c>
       <c r="C16" s="59" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="F16" s="59" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="G16" s="59" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="63"/>
@@ -8679,19 +8679,19 @@
         <v>51</v>
       </c>
       <c r="C17" s="59" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="E17" s="59" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="F17" s="59" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="G17" s="59" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="63"/>
@@ -8704,19 +8704,19 @@
         <v>51</v>
       </c>
       <c r="C18" s="59" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E18" s="59" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="F18" s="59" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G18" s="59" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="63"/>
@@ -8729,19 +8729,19 @@
         <v>51</v>
       </c>
       <c r="C19" s="59" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E19" s="59" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="F19" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="59" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="63"/>
@@ -8778,8 +8778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BB51EF-9754-4843-8AC4-284490EA6437}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -8798,7 +8798,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8811,7 +8811,7 @@
     </row>
     <row r="2" spans="1:9" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -8824,7 +8824,7 @@
     </row>
     <row r="3" spans="1:9" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -8865,7 +8865,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="73" t="s">
-        <v>476</v>
+        <v>461</v>
       </c>
       <c r="G5" s="73" t="s">
         <v>7</v>
@@ -8885,19 +8885,19 @@
         <v>51</v>
       </c>
       <c r="C6" s="59" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>523</v>
+        <v>500</v>
       </c>
       <c r="F6" s="59" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="59" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="H6" s="59"/>
       <c r="I6" s="63"/>
@@ -8932,13 +8932,13 @@
         <v>6</v>
       </c>
       <c r="F8" s="73" t="s">
-        <v>475</v>
+        <v>460</v>
       </c>
       <c r="G8" s="73" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="73" t="s">
-        <v>477</v>
+        <v>462</v>
       </c>
       <c r="I8" s="73" t="s">
         <v>52</v>
@@ -8952,19 +8952,19 @@
         <v>51</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F9" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G9" s="59" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="H9" s="57"/>
       <c r="I9" s="63"/>
@@ -8977,19 +8977,19 @@
         <v>51</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="E10" s="59" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F10" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="59" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="H10" s="57"/>
       <c r="I10" s="63"/>
@@ -9002,19 +9002,19 @@
         <v>51</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E11" s="59" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F11" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="59" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H11" s="57"/>
       <c r="I11" s="63"/>
@@ -9027,19 +9027,19 @@
         <v>51</v>
       </c>
       <c r="C12" s="59" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E12" s="59" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="F12" s="59" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G12" s="59" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="H12" s="57"/>
       <c r="I12" s="63"/>
@@ -9052,19 +9052,19 @@
         <v>51</v>
       </c>
       <c r="C13" s="59" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="E13" s="59" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="F13" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="H13" s="57"/>
       <c r="I13" s="63"/>
@@ -9076,16 +9076,16 @@
       </c>
       <c r="C14" s="59"/>
       <c r="D14" s="64" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="E14" s="59" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="F14" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="H14" s="57"/>
       <c r="I14" s="63"/>
@@ -9097,16 +9097,16 @@
       </c>
       <c r="C15" s="59"/>
       <c r="D15" s="64" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="E15" s="59" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="F15" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G15" s="59" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="H15" s="57"/>
       <c r="I15" s="63"/>
@@ -9119,40 +9119,40 @@
         <v>51</v>
       </c>
       <c r="C16" s="59" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="E16" s="59" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="F16" s="59" t="s">
         <v>90</v>
       </c>
       <c r="G16" s="59" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="H16" s="57"/>
       <c r="I16" s="63"/>
     </row>
-    <row r="17" spans="1:9" ht="217" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="232.5" x14ac:dyDescent="0.35">
       <c r="A17" s="92"/>
       <c r="B17" s="61" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="59"/>
       <c r="D17" s="64" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="E17" s="59" t="s">
-        <v>511</v>
+        <v>492</v>
       </c>
       <c r="F17" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="59" t="s">
-        <v>512</v>
+        <v>493</v>
       </c>
       <c r="H17" s="57"/>
       <c r="I17" s="63"/>

</xml_diff>